<commit_message>
Se agrego la consulta de las lines en sql
</commit_message>
<xml_diff>
--- a/Variables FACTURA GRAVADA.xlsx
+++ b/Variables FACTURA GRAVADA.xlsx
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E48"/>
+  <dimension ref="A2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E48"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
     <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -535,8 +535,12 @@
         <f>CONCATENATE(A2," ",B2," (",C2,")")</f>
         <v>operacion nchar (12)</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f>"("&amp;"'"&amp;A2&amp;"'"&amp;")"&amp;","</f>
+        <v>('operacion'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -551,8 +555,12 @@
         <f>CONCATENATE(A3," ",B3," (",C3,")",",")</f>
         <v>tipo_de_comprobante Integer  (),</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H48" si="1">"("&amp;"'"&amp;A3&amp;"'"&amp;")"&amp;","</f>
+        <v>('tipo_de_comprobante'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -567,11 +575,15 @@
         <v>DECLARE @serie nchar (4)</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E48" si="1">CONCATENATE(A4," ",B4," (",C4,")",",")</f>
+        <f t="shared" ref="E4:E48" si="2">CONCATENATE(A4," ",B4," (",C4,")",",")</f>
         <v>serie nchar (4),</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>('serie'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -583,11 +595,15 @@
         <v>DECLARE @numero Integer  ()</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>numero Integer  (),</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>('numero'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -599,11 +615,15 @@
         <v>DECLARE @sunat_transaction Integer  ()</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>sunat_transaction Integer  (),</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>('sunat_transaction'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -615,11 +635,15 @@
         <v>DECLARE @cliente_tipo_de_documento Integer  ()</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cliente_tipo_de_documento Integer  (),</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>('cliente_tipo_de_documento'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -634,11 +658,15 @@
         <v>DECLARE @cliente_numero_de_documento nchar (15)</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cliente_numero_de_documento nchar (15),</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>('cliente_numero_de_documento'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -653,11 +681,15 @@
         <v>DECLARE @cliente_denominacion nvarchar (100)</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cliente_denominacion nvarchar (100),</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>('cliente_denominacion'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -672,11 +704,15 @@
         <v>DECLARE @cliente_direccion nvarchar (100)</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cliente_direccion nvarchar (100),</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>('cliente_direccion'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -691,11 +727,15 @@
         <v>DECLARE @cliente_email nvarchar (250)</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cliente_email nvarchar (250),</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>('cliente_email'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -710,11 +750,15 @@
         <v>DECLARE @cliente_email_1 nvarchar (250)</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cliente_email_1 nvarchar (250),</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>('cliente_email_1'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -729,11 +773,15 @@
         <v>DECLARE @cliente_email_2 nvarchar (250)</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cliente_email_2 nvarchar (250),</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>('cliente_email_2'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -748,11 +796,15 @@
         <v>DECLARE @fecha_de_emision date (10)</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>fecha_de_emision date (10),</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>('fecha_de_emision'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -767,11 +819,15 @@
         <v>DECLARE @fecha_de_vencimiento date (10)</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>fecha_de_vencimiento date (10),</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>('fecha_de_vencimiento'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -783,11 +839,15 @@
         <v>DECLARE @moneda Integer  ()</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>moneda Integer  (),</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>('moneda'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -802,11 +862,15 @@
         <v>DECLARE @tipo_de_cambio numeric (2,2)</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>tipo_de_cambio numeric (2,2),</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>('tipo_de_cambio'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -821,11 +885,15 @@
         <v>DECLARE @porcentaje_de_igv numeric (2,2)</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>porcentaje_de_igv numeric (2,2),</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>('porcentaje_de_igv'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -840,11 +908,15 @@
         <v>DECLARE @descuento_global numeric (12,2)</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>descuento_global numeric (12,2),</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>('descuento_global'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -859,11 +931,15 @@
         <v>DECLARE @total_descuento numeric (12,2)</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_descuento numeric (12,2),</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_descuento'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -878,11 +954,15 @@
         <v>DECLARE @total_anticipo numeric (12,2)</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_anticipo numeric (12,2),</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_anticipo'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -897,11 +977,15 @@
         <v>DECLARE @total_gravada numeric (12,2)</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_gravada numeric (12,2),</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_gravada'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -916,11 +1000,15 @@
         <v>DECLARE @total_inafecta numeric (12,2)</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_inafecta numeric (12,2),</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_inafecta'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -935,11 +1023,15 @@
         <v>DECLARE @total_exonerada numeric (12,2)</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_exonerada numeric (12,2),</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_exonerada'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -954,11 +1046,15 @@
         <v>DECLARE @total_igv numeric (12,2)</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_igv numeric (12,2),</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_igv'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -973,11 +1069,15 @@
         <v>DECLARE @total_gratuita numeric (12,2)</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_gratuita numeric (12,2),</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_gratuita'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -992,11 +1092,15 @@
         <v>DECLARE @total_otros_cargos numeric (12,2)</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_otros_cargos numeric (12,2),</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_otros_cargos'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1011,11 +1115,15 @@
         <v>DECLARE @total numeric (12,2)</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total numeric (12,2),</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>('total'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1027,11 +1135,15 @@
         <v>DECLARE @percepcion_tipo Integer  ()</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>percepcion_tipo Integer  (),</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>('percepcion_tipo'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1046,11 +1158,15 @@
         <v>DECLARE @percepcion_base_imponible numeric (12,2)</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>percepcion_base_imponible numeric (12,2),</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>('percepcion_base_imponible'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1065,11 +1181,15 @@
         <v>DECLARE @total_percepcion numeric (12,2)</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_percepcion numeric (12,2),</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_percepcion'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1084,11 +1204,15 @@
         <v>DECLARE @total_incluido_percepcion numeric (12,2)</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>total_incluido_percepcion numeric (12,2),</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>('total_incluido_percepcion'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1103,11 +1227,15 @@
         <v>DECLARE @detraccion nchar (5)</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>detraccion nchar (5),</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>('detraccion'),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1122,11 +1250,15 @@
         <v>DECLARE @observaciones nvarchar (5)</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>observaciones nvarchar (5),</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>('observaciones'),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1138,11 +1270,15 @@
         <v>DECLARE @documento_que_se_modifica_tipo Integer  ()</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>documento_que_se_modifica_tipo Integer  (),</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v>('documento_que_se_modifica_tipo'),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1157,11 +1293,15 @@
         <v>DECLARE @documento_que_se_modifica_serie nchar (4)</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>documento_que_se_modifica_serie nchar (4),</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v>('documento_que_se_modifica_serie'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1176,11 +1316,15 @@
         <v>DECLARE @documento_que_se_modifica_numero nchar (8)</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>documento_que_se_modifica_numero nchar (8),</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v>('documento_que_se_modifica_numero'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1192,11 +1336,15 @@
         <v>DECLARE @tipo_de_nota_de_credito Integer  ()</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>tipo_de_nota_de_credito Integer  (),</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" t="str">
+        <f t="shared" si="1"/>
+        <v>('tipo_de_nota_de_credito'),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1208,11 +1356,15 @@
         <v>DECLARE @tipo_de_nota_de_debito Integer  ()</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>tipo_de_nota_de_debito Integer  (),</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" t="str">
+        <f t="shared" si="1"/>
+        <v>('tipo_de_nota_de_debito'),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1227,11 +1379,15 @@
         <v>DECLARE @enviar_automaticamente_a_la_sunat nchar (5)</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>enviar_automaticamente_a_la_sunat nchar (5),</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" t="str">
+        <f t="shared" si="1"/>
+        <v>('enviar_automaticamente_a_la_sunat'),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1246,11 +1402,15 @@
         <v>DECLARE @enviar_automaticamente_al_cliente nchar (5)</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>enviar_automaticamente_al_cliente nchar (5),</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" t="str">
+        <f t="shared" si="1"/>
+        <v>('enviar_automaticamente_al_cliente'),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1265,11 +1425,15 @@
         <v>DECLARE @codigo_unico nvarchar (20)</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>codigo_unico nvarchar (20),</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" t="str">
+        <f t="shared" si="1"/>
+        <v>('codigo_unico'),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1284,11 +1448,15 @@
         <v>DECLARE @condiciones_de_pago nvarchar (250)</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>condiciones_de_pago nvarchar (250),</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" t="str">
+        <f t="shared" si="1"/>
+        <v>('condiciones_de_pago'),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1303,11 +1471,15 @@
         <v>DECLARE @medio_de_pago nvarchar (250)</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>medio_de_pago nvarchar (250),</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" t="str">
+        <f t="shared" si="1"/>
+        <v>('medio_de_pago'),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1322,11 +1494,15 @@
         <v>DECLARE @placa_vehiculo nvarchar (8)</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>placa_vehiculo nvarchar (8),</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v>('placa_vehiculo'),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1341,11 +1517,15 @@
         <v>DECLARE @orden_compra_servicio nvarchar (20)</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>orden_compra_servicio nvarchar (20),</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" t="str">
+        <f t="shared" si="1"/>
+        <v>('orden_compra_servicio'),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1360,11 +1540,15 @@
         <v>DECLARE @tabla_personalizada_codigo nvarchar (250)</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>tabla_personalizada_codigo nvarchar (250),</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" t="str">
+        <f t="shared" si="1"/>
+        <v>('tabla_personalizada_codigo'),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1379,8 +1563,12 @@
         <v>DECLARE @formato_de_pdf nvarchar (5)</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>formato_de_pdf nvarchar (5),</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="1"/>
+        <v>('formato_de_pdf'),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>